<commit_message>
Minor Edit to Assest List
Joy did a fantastic job with the assest list, very thankful for their hard week. I know we can get way more done, but these are the bare essentials for the game. In addition, life happens. This game isn't a dedicated project, it's for a class. Of course, we're going to elevate the concept and make it awesome, but it's not a guaranteed time commitment. I want to focus on finished and functional before worrying about putting out the next big hit.
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DarkRoot\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wolff\OneDrive\Documents\DarkRootV3\DarkRoot\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673BEA44-06E3-4412-9D97-67875AC7F46A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91822C13-71D4-4434-83A2-DAD70061065F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83EF7ABD-5B94-4EE7-81F2-F128B123CE05}"/>
+    <workbookView xWindow="4940" yWindow="4940" windowWidth="28800" windowHeight="15460" xr2:uid="{83EF7ABD-5B94-4EE7-81F2-F128B123CE05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="103">
   <si>
     <t>Asset</t>
   </si>
@@ -341,6 +330,12 @@
   </si>
   <si>
     <t>Enemy bullets slower, more distinct color. Better chance for Player to dodge.</t>
+  </si>
+  <si>
+    <t>Ultimate Carrot Cannon</t>
+  </si>
+  <si>
+    <t>The end game weapon, Carrot Quest's master sword. A sacred weapon</t>
   </si>
 </sst>
 </file>
@@ -497,13 +492,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -549,8 +544,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC7CCED1-F0DA-4309-901B-2344FEB332E5}" name="Table1" displayName="Table1" ref="B3:H59" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B3:H59" xr:uid="{CC7CCED1-F0DA-4309-901B-2344FEB332E5}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC7CCED1-F0DA-4309-901B-2344FEB332E5}" name="Table1" displayName="Table1" ref="B3:H61" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B3:H61" xr:uid="{CC7CCED1-F0DA-4309-901B-2344FEB332E5}"/>
   <tableColumns count="7">
     <tableColumn id="13" xr3:uid="{AF7E0E7C-2284-413F-AB2C-E63BCFCC2C85}" name="Department"/>
     <tableColumn id="1" xr3:uid="{4F89ED6B-F192-4EF7-BB55-9FBCF02369DF}" name="Asset"/>
@@ -861,38 +856,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C743A33-A4BC-416E-821B-F9208C97A8E0}">
-  <dimension ref="B2:J59"/>
+  <dimension ref="B2:J61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
-    <col min="4" max="4" width="85.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.21875" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="11.21875" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" customWidth="1"/>
+    <col min="4" max="4" width="85.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" customWidth="1"/>
+    <col min="7" max="7" width="12.453125" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" customWidth="1"/>
+    <col min="9" max="9" width="11.6328125" customWidth="1"/>
+    <col min="10" max="10" width="11.1796875" customWidth="1"/>
+    <col min="11" max="11" width="11.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="2:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+    </row>
+    <row r="3" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
@@ -918,8 +913,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C4" t="s">
@@ -944,8 +939,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C5" t="s">
@@ -970,8 +965,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B6" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
@@ -996,8 +991,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B7" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C7" t="s">
@@ -1019,8 +1014,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="9" t="s">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C8" t="s">
@@ -1042,8 +1037,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="9" t="s">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C9" t="s">
@@ -1065,8 +1060,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C10" t="s">
@@ -1088,8 +1083,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="9" t="s">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C11" t="s">
@@ -1111,8 +1106,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B12" s="9" t="s">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C12" t="s">
@@ -1134,8 +1129,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B13" s="9" t="s">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B13" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C13" t="s">
@@ -1157,8 +1152,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="9" t="s">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C14" t="s">
@@ -1180,8 +1175,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="9" t="s">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C15" t="s">
@@ -1203,8 +1198,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="9" t="s">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C16" t="s">
@@ -1226,8 +1221,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B17" s="9" t="s">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C17" t="s">
@@ -1249,8 +1244,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B18" s="9" t="s">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C18" t="s">
@@ -1272,8 +1267,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B19" s="9" t="s">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C19" t="s">
@@ -1295,8 +1290,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B20" s="9" t="s">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C20" t="s">
@@ -1318,8 +1313,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B21" s="9" t="s">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C21" t="s">
@@ -1341,8 +1336,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B22" s="9" t="s">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B22" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C22" t="s">
@@ -1364,8 +1359,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B23" s="9" t="s">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B23" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C23" t="s">
@@ -1387,8 +1382,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B24" s="9" t="s">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C24" t="s">
@@ -1410,8 +1405,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B25" s="9" t="s">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C25" t="s">
@@ -1433,8 +1428,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B26" s="9" t="s">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C26" t="s">
@@ -1456,8 +1451,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B27" s="9" t="s">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C27" t="s">
@@ -1479,8 +1474,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B28" s="9" t="s">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C28" t="s">
@@ -1502,8 +1497,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B29" s="9" t="s">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C29" t="s">
@@ -1525,8 +1520,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B30" s="9" t="s">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C30" t="s">
@@ -1548,8 +1543,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B31" s="9" t="s">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B31" s="8" t="s">
         <v>24</v>
       </c>
       <c r="C31" t="s">
@@ -1571,11 +1566,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H32" s="12"/>
-    </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B33" s="10" t="s">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H32" s="11"/>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B33" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C33" t="s">
@@ -1597,8 +1592,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="10" t="s">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B34" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C34" t="s">
@@ -1620,8 +1615,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B35" s="10" t="s">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B35" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C35" t="s">
@@ -1643,8 +1638,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B36" s="10" t="s">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B36" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C36" t="s">
@@ -1666,8 +1661,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="10" t="s">
+    <row r="37" spans="2:8" ht="28.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C37" t="s">
@@ -1689,8 +1684,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B38" s="10" t="s">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B38" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C38" t="s">
@@ -1712,8 +1707,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B39" s="10" t="s">
+    <row r="39" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="B39" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C39" t="s">
@@ -1735,8 +1730,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B40" s="10" t="s">
+    <row r="40" spans="2:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="B40" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C40" t="s">
@@ -1758,8 +1753,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="10" t="s">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C41" t="s">
@@ -1781,8 +1776,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B42" s="10" t="s">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B42" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C42" t="s">
@@ -1804,8 +1799,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B43" s="10" t="s">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C43" t="s">
@@ -1827,8 +1822,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B44" s="10" t="s">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C44" t="s">
@@ -1850,8 +1845,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B45" s="10" t="s">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B45" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C45" t="s">
@@ -1873,8 +1868,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B46" s="10" t="s">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B46" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C46" t="s">
@@ -1896,8 +1891,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B47" s="10" t="s">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B47" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C47" t="s">
@@ -1919,21 +1914,21 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B48" s="10" t="s">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B48" s="9" t="s">
         <v>40</v>
       </c>
       <c r="C48" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D48" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="E48" t="s">
         <v>43</v>
       </c>
       <c r="F48" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G48" t="s">
         <v>30</v>
@@ -1942,110 +1937,104 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H49" s="12"/>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B50" s="11" t="s">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B49" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" t="s">
+        <v>43</v>
+      </c>
+      <c r="F49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G49" t="s">
+        <v>30</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B50" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" t="s">
+        <v>100</v>
+      </c>
+      <c r="E50" t="s">
+        <v>43</v>
+      </c>
+      <c r="F50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" t="s">
+        <v>30</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="H51" s="11"/>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B52" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>69</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D52" t="s">
         <v>71</v>
       </c>
-      <c r="E50" t="s">
-        <v>43</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="E52" t="s">
+        <v>43</v>
+      </c>
+      <c r="F52" t="s">
         <v>9</v>
       </c>
-      <c r="G50" t="s">
-        <v>22</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B51" s="11" t="s">
+      <c r="G52" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B53" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C53" t="s">
         <v>70</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D53" t="s">
         <v>72</v>
       </c>
-      <c r="E51" t="s">
-        <v>43</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="E53" t="s">
+        <v>43</v>
+      </c>
+      <c r="F53" t="s">
         <v>9</v>
       </c>
-      <c r="G51" t="s">
-        <v>22</v>
-      </c>
-      <c r="H51" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B52" s="11" t="s">
+      <c r="G53" t="s">
+        <v>22</v>
+      </c>
+      <c r="H53" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C54" t="s">
         <v>73</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D54" t="s">
         <v>75</v>
-      </c>
-      <c r="E52" t="s">
-        <v>43</v>
-      </c>
-      <c r="F52" t="s">
-        <v>12</v>
-      </c>
-      <c r="G52" t="s">
-        <v>22</v>
-      </c>
-      <c r="H52" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B53" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C53" t="s">
-        <v>74</v>
-      </c>
-      <c r="D53" t="s">
-        <v>76</v>
-      </c>
-      <c r="E53" t="s">
-        <v>43</v>
-      </c>
-      <c r="F53" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" t="s">
-        <v>22</v>
-      </c>
-      <c r="H53" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B54" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C54" t="s">
-        <v>78</v>
-      </c>
-      <c r="D54" t="s">
-        <v>77</v>
       </c>
       <c r="E54" t="s">
         <v>43</v>
@@ -2054,27 +2043,27 @@
         <v>12</v>
       </c>
       <c r="G54" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="H54" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B55" s="11" t="s">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C55" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D55" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E55" t="s">
         <v>43</v>
       </c>
       <c r="F55" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G55" t="s">
         <v>22</v>
@@ -2083,8 +2072,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B56" s="11" t="s">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B56" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C56" t="s">
@@ -2097,7 +2086,7 @@
         <v>43</v>
       </c>
       <c r="F56" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="G56" t="s">
         <v>30</v>
@@ -2106,38 +2095,38 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B57" s="11" t="s">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B57" s="10" t="s">
         <v>68</v>
       </c>
       <c r="C57" t="s">
+        <v>79</v>
+      </c>
+      <c r="D57" t="s">
+        <v>80</v>
+      </c>
+      <c r="E57" t="s">
+        <v>43</v>
+      </c>
+      <c r="F57" t="s">
+        <v>13</v>
+      </c>
+      <c r="G57" t="s">
+        <v>22</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B58" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C58" t="s">
         <v>78</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D58" t="s">
         <v>77</v>
-      </c>
-      <c r="E57" t="s">
-        <v>43</v>
-      </c>
-      <c r="F57" t="s">
-        <v>15</v>
-      </c>
-      <c r="G57" t="s">
-        <v>30</v>
-      </c>
-      <c r="H57" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B58" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="C58" t="s">
-        <v>83</v>
-      </c>
-      <c r="D58" t="s">
-        <v>84</v>
       </c>
       <c r="E58" t="s">
         <v>43</v>
@@ -2152,9 +2141,55 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B59" s="11"/>
-      <c r="H59" s="2"/>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B59" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" t="s">
+        <v>78</v>
+      </c>
+      <c r="D59" t="s">
+        <v>77</v>
+      </c>
+      <c r="E59" t="s">
+        <v>43</v>
+      </c>
+      <c r="F59" t="s">
+        <v>15</v>
+      </c>
+      <c r="G59" t="s">
+        <v>30</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B60" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C60" t="s">
+        <v>83</v>
+      </c>
+      <c r="D60" t="s">
+        <v>84</v>
+      </c>
+      <c r="E60" t="s">
+        <v>43</v>
+      </c>
+      <c r="F60" t="s">
+        <v>15</v>
+      </c>
+      <c r="G60" t="s">
+        <v>30</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B61" s="10"/>
+      <c r="H61" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
A few minor doc updates
minor tweaks to documentation before submitting
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DarkRoot\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B20971-7438-4DA7-9B88-B405D10A49BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{532771C8-3A5B-405B-AAFA-CB22E027A5AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83EF7ABD-5B94-4EE7-81F2-F128B123CE05}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="124">
   <si>
     <t>Asset</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Week 6</t>
-  </si>
-  <si>
-    <t>Week 7</t>
   </si>
   <si>
     <t>Week 8</t>
@@ -411,6 +408,9 @@
   </si>
   <si>
     <t>Incomplete 80%</t>
+  </si>
+  <si>
+    <t>On Hold</t>
   </si>
 </sst>
 </file>
@@ -941,7 +941,7 @@
   <dimension ref="B2:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,7 +971,7 @@
     </row>
     <row r="3" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -992,660 +992,660 @@
         <v>5</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
       <c r="E7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="C9" t="s">
-        <v>25</v>
-      </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
       <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" t="s">
         <v>29</v>
       </c>
-      <c r="E10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
         <v>35</v>
       </c>
-      <c r="D11" t="s">
-        <v>36</v>
-      </c>
       <c r="E11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F20" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F21" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
         <v>38</v>
       </c>
-      <c r="D23" t="s">
-        <v>39</v>
-      </c>
       <c r="E23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
         <v>81</v>
       </c>
-      <c r="D24" t="s">
-        <v>82</v>
-      </c>
       <c r="E24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D25" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E25" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D26" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E26" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F26" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F27" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F28" t="s">
         <v>14</v>
       </c>
       <c r="G28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E29" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F29" t="s">
         <v>14</v>
       </c>
       <c r="G29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C30" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" t="s">
         <v>95</v>
       </c>
-      <c r="D30" t="s">
-        <v>96</v>
-      </c>
       <c r="E30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E31" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.3">
@@ -1653,416 +1653,416 @@
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
         <v>40</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
         <v>41</v>
       </c>
-      <c r="D33" t="s">
-        <v>42</v>
-      </c>
       <c r="E33" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F33" t="s">
         <v>7</v>
       </c>
       <c r="G33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>18</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
       </c>
       <c r="G34" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" t="s">
         <v>47</v>
       </c>
-      <c r="D35" t="s">
-        <v>48</v>
-      </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
       </c>
       <c r="G35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="D36" s="7" t="s">
-        <v>105</v>
-      </c>
       <c r="E36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F36" t="s">
         <v>9</v>
       </c>
       <c r="G36" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="37" spans="2:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F37" t="s">
         <v>9</v>
       </c>
       <c r="G37" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="38" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B38" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E38" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F38" t="s">
         <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B39" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D39" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E39" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
       </c>
       <c r="G39" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B40" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E41" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F41" t="s">
         <v>11</v>
       </c>
       <c r="G41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F42" t="s">
         <v>11</v>
       </c>
       <c r="G42" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B43" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E43" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F43" t="s">
         <v>11</v>
       </c>
       <c r="G43" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D44" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E44" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F44" t="s">
         <v>12</v>
       </c>
       <c r="G44" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B45" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D45" t="s">
         <v>58</v>
       </c>
-      <c r="D45" t="s">
-        <v>59</v>
-      </c>
       <c r="E45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F45" t="s">
         <v>12</v>
       </c>
       <c r="G45" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B46" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
+        <v>60</v>
+      </c>
+      <c r="D46" t="s">
         <v>61</v>
       </c>
-      <c r="D46" t="s">
-        <v>62</v>
-      </c>
       <c r="E46" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F47" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G47" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B48" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" t="s">
         <v>64</v>
       </c>
-      <c r="D48" t="s">
-        <v>65</v>
-      </c>
       <c r="E48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G48" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B49" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
+        <v>65</v>
+      </c>
+      <c r="D49" t="s">
         <v>66</v>
       </c>
-      <c r="D49" t="s">
-        <v>67</v>
-      </c>
       <c r="E49" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G49" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" t="s">
         <v>99</v>
       </c>
-      <c r="D50" t="s">
-        <v>100</v>
-      </c>
       <c r="E50" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F50" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.3">
@@ -2070,278 +2070,278 @@
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B52" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C52" t="s">
         <v>68</v>
       </c>
-      <c r="C52" t="s">
-        <v>69</v>
-      </c>
       <c r="D52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F52" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G52" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B53" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F53" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G53" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C54" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" t="s">
         <v>110</v>
       </c>
-      <c r="D54" t="s">
-        <v>111</v>
-      </c>
       <c r="E54" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F54" t="s">
         <v>10</v>
       </c>
       <c r="G54" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B55" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C55" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" t="s">
         <v>106</v>
       </c>
-      <c r="D55" t="s">
-        <v>107</v>
-      </c>
       <c r="E55" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F55" t="s">
         <v>10</v>
       </c>
       <c r="G55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C56" t="s">
+        <v>107</v>
+      </c>
+      <c r="D56" t="s">
         <v>108</v>
       </c>
-      <c r="D56" t="s">
-        <v>109</v>
-      </c>
       <c r="E56" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F56" t="s">
         <v>11</v>
       </c>
       <c r="G56" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H56" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C57" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" t="s">
         <v>112</v>
       </c>
-      <c r="D57" t="s">
-        <v>113</v>
-      </c>
       <c r="E57" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F57" t="s">
         <v>11</v>
       </c>
       <c r="G57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D58" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E58" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G58" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B59" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D59" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E59" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F59" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G59" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C60" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D60" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E60" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G60" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B61" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C61" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" t="s">
         <v>79</v>
       </c>
-      <c r="D61" t="s">
-        <v>80</v>
-      </c>
       <c r="E61" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G61" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B62" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C62" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" t="s">
         <v>101</v>
       </c>
-      <c r="D62" t="s">
-        <v>102</v>
-      </c>
       <c r="E62" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G62" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B63" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C63" t="s">
+        <v>82</v>
+      </c>
+      <c r="D63" t="s">
         <v>83</v>
       </c>
-      <c r="D63" t="s">
-        <v>84</v>
-      </c>
       <c r="E63" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F63" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G63" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.3">
@@ -2349,85 +2349,82 @@
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B65" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C65" t="s">
         <v>114</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>115</v>
-      </c>
-      <c r="D65" t="s">
-        <v>116</v>
-      </c>
-      <c r="E65" t="s">
-        <v>17</v>
       </c>
       <c r="F65" t="s">
         <v>8</v>
       </c>
       <c r="G65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B66" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C66" t="s">
+        <v>116</v>
+      </c>
+      <c r="D66" t="s">
         <v>117</v>
       </c>
-      <c r="D66" t="s">
-        <v>118</v>
-      </c>
       <c r="F66" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G66" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B67" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C67" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F67" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G67" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B68" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C68" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D68" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F68" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G68" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Slime spritesheets & update asset list
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FroggyChainsaw\Documents\GitHub\DarkRoot\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DarkRoot\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CE4056-4F84-4EA7-AA30-D55788D48D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E68D20-556A-445F-8D0E-AD3627FBA982}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{83EF7ABD-5B94-4EE7-81F2-F128B123CE05}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{83EF7ABD-5B94-4EE7-81F2-F128B123CE05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="129">
   <si>
     <t>Asset</t>
   </si>
@@ -408,6 +408,24 @@
   </si>
   <si>
     <t>Complete 80%</t>
+  </si>
+  <si>
+    <t>ON HOLD</t>
+  </si>
+  <si>
+    <t>Incomplete 80%</t>
+  </si>
+  <si>
+    <t>Currently auto-pickup instead of press E</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Incomplete 99%</t>
+  </si>
+  <si>
+    <t>This used to work but now doesn't?</t>
   </si>
 </sst>
 </file>
@@ -474,7 +492,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -526,6 +544,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -557,7 +581,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -575,10 +599,11 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -609,6 +634,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFBB779"/>
+      <color rgb="FFFFDE75"/>
       <color rgb="FFDEC8EE"/>
     </mruColors>
   </colors>
@@ -624,9 +651,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC7CCED1-F0DA-4309-901B-2344FEB332E5}" name="Table1" displayName="Table1" ref="B3:H69" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B3:H69" xr:uid="{CC7CCED1-F0DA-4309-901B-2344FEB332E5}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CC7CCED1-F0DA-4309-901B-2344FEB332E5}" name="Table1" displayName="Table1" ref="B3:I69" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="B3:I69" xr:uid="{CC7CCED1-F0DA-4309-901B-2344FEB332E5}"/>
+  <tableColumns count="8">
     <tableColumn id="13" xr3:uid="{AF7E0E7C-2284-413F-AB2C-E63BCFCC2C85}" name="Department"/>
     <tableColumn id="1" xr3:uid="{4F89ED6B-F192-4EF7-BB55-9FBCF02369DF}" name="Asset"/>
     <tableColumn id="2" xr3:uid="{EDE03673-BD30-4FF7-B06B-A15B43AFBEE4}" name="Task"/>
@@ -634,6 +661,7 @@
     <tableColumn id="4" xr3:uid="{052CDE0A-BEBF-4108-8152-B47C430A4FED}" name="Due"/>
     <tableColumn id="5" xr3:uid="{A5F33B29-DA99-4349-8327-5E8371464113}" name="Priority"/>
     <tableColumn id="6" xr3:uid="{9AF1C154-CE0B-4738-A496-995DBF943D11}" name="Status"/>
+    <tableColumn id="7" xr3:uid="{E492A22D-4DD5-420C-85B7-44777415B9B5}" name="Comments"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -938,36 +966,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C743A33-A4BC-416E-821B-F9208C97A8E0}">
   <dimension ref="B2:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="3" width="21.7109375" customWidth="1"/>
-    <col min="4" max="4" width="85.7109375" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="85.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="33.5546875" customWidth="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="B2" s="13" t="s">
+    <row r="2" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="B2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-    </row>
-    <row r="3" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+    </row>
+    <row r="3" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -989,11 +1017,14 @@
       <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="I3" s="1" t="s">
+        <v>126</v>
+      </c>
       <c r="J3" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B4" s="8" t="s">
         <v>23</v>
       </c>
@@ -1019,7 +1050,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B5" s="8" t="s">
         <v>23</v>
       </c>
@@ -1045,7 +1076,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8" t="s">
         <v>23</v>
       </c>
@@ -1071,7 +1102,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
@@ -1090,11 +1121,11 @@
       <c r="G7" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" s="8" t="s">
         <v>23</v>
       </c>
@@ -1113,11 +1144,11 @@
       <c r="G8" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B9" s="8" t="s">
         <v>23</v>
       </c>
@@ -1136,11 +1167,11 @@
       <c r="G9" t="s">
         <v>21</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" s="8" t="s">
         <v>23</v>
       </c>
@@ -1159,11 +1190,11 @@
       <c r="G10" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H10" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>23</v>
       </c>
@@ -1180,13 +1211,13 @@
         <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>23</v>
       </c>
@@ -1205,11 +1236,11 @@
       <c r="G12" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" s="8" t="s">
         <v>23</v>
       </c>
@@ -1228,11 +1259,11 @@
       <c r="G13" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>23</v>
       </c>
@@ -1251,11 +1282,11 @@
       <c r="G14" t="s">
         <v>21</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
         <v>23</v>
       </c>
@@ -1272,13 +1303,13 @@
         <v>11</v>
       </c>
       <c r="G15" t="s">
-        <v>21</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>23</v>
       </c>
@@ -1297,11 +1328,11 @@
       <c r="G16" t="s">
         <v>21</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H16" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="8" t="s">
         <v>23</v>
       </c>
@@ -1320,11 +1351,11 @@
       <c r="G17" t="s">
         <v>21</v>
       </c>
-      <c r="H17" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H17" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B18" s="8" t="s">
         <v>23</v>
       </c>
@@ -1343,11 +1374,11 @@
       <c r="G18" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H18" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>23</v>
       </c>
@@ -1366,11 +1397,11 @@
       <c r="G19" t="s">
         <v>21</v>
       </c>
-      <c r="H19" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B20" s="8" t="s">
         <v>23</v>
       </c>
@@ -1389,11 +1420,11 @@
       <c r="G20" t="s">
         <v>21</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H20" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>23</v>
       </c>
@@ -1412,11 +1443,11 @@
       <c r="G21" t="s">
         <v>21</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H21" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B22" s="8" t="s">
         <v>23</v>
       </c>
@@ -1435,11 +1466,11 @@
       <c r="G22" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H22" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="8" t="s">
         <v>23</v>
       </c>
@@ -1458,11 +1489,11 @@
       <c r="G23" t="s">
         <v>21</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H23" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B24" s="8" t="s">
         <v>23</v>
       </c>
@@ -1481,11 +1512,11 @@
       <c r="G24" t="s">
         <v>29</v>
       </c>
-      <c r="H24" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H24" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B25" s="8" t="s">
         <v>23</v>
       </c>
@@ -1508,7 +1539,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B26" s="8" t="s">
         <v>23</v>
       </c>
@@ -1531,7 +1562,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B27" s="8" t="s">
         <v>23</v>
       </c>
@@ -1554,7 +1585,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B28" s="8" t="s">
         <v>23</v>
       </c>
@@ -1573,11 +1604,11 @@
       <c r="G28" t="s">
         <v>29</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H28" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B29" s="8" t="s">
         <v>23</v>
       </c>
@@ -1596,11 +1627,11 @@
       <c r="G29" t="s">
         <v>29</v>
       </c>
-      <c r="H29" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B30" s="8" t="s">
         <v>23</v>
       </c>
@@ -1623,7 +1654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
         <v>23</v>
       </c>
@@ -1642,14 +1673,14 @@
       <c r="G31" t="s">
         <v>29</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H31" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H32" s="11"/>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="9" t="s">
         <v>39</v>
       </c>
@@ -1668,11 +1699,11 @@
       <c r="G33" t="s">
         <v>29</v>
       </c>
-      <c r="H33" s="14" t="s">
+      <c r="H33" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="9" t="s">
         <v>39</v>
       </c>
@@ -1695,7 +1726,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="9" t="s">
         <v>39</v>
       </c>
@@ -1718,7 +1749,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B36" s="9" t="s">
         <v>39</v>
       </c>
@@ -1741,7 +1772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:9" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B37" s="9" t="s">
         <v>39</v>
       </c>
@@ -1764,7 +1795,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="38" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B38" s="9" t="s">
         <v>39</v>
       </c>
@@ -1783,11 +1814,11 @@
       <c r="G38" t="s">
         <v>21</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H38" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B39" s="9" t="s">
         <v>39</v>
       </c>
@@ -1806,11 +1837,11 @@
       <c r="G39" t="s">
         <v>21</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H39" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B40" s="9" t="s">
         <v>39</v>
       </c>
@@ -1829,11 +1860,11 @@
       <c r="G40" t="s">
         <v>21</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="41" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H40" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B41" s="9" t="s">
         <v>39</v>
       </c>
@@ -1853,10 +1884,10 @@
         <v>21</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
         <v>39</v>
       </c>
@@ -1879,7 +1910,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B43" s="9" t="s">
         <v>39</v>
       </c>
@@ -1902,7 +1933,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" s="9" t="s">
         <v>39</v>
       </c>
@@ -1922,10 +1953,13 @@
         <v>21</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="I44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B45" s="9" t="s">
         <v>39</v>
       </c>
@@ -1948,7 +1982,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B46" s="9" t="s">
         <v>39</v>
       </c>
@@ -1971,7 +2005,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B47" s="9" t="s">
         <v>39</v>
       </c>
@@ -1994,7 +2028,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B48" s="9" t="s">
         <v>39</v>
       </c>
@@ -2017,7 +2051,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B49" s="9" t="s">
         <v>39</v>
       </c>
@@ -2040,7 +2074,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="9" t="s">
         <v>39</v>
       </c>
@@ -2063,10 +2097,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H51" s="11"/>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B52" s="10" t="s">
         <v>67</v>
       </c>
@@ -2089,7 +2123,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" s="10" t="s">
         <v>67</v>
       </c>
@@ -2106,13 +2140,13 @@
         <v>10</v>
       </c>
       <c r="G53" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B54" s="10" t="s">
         <v>67</v>
       </c>
@@ -2132,10 +2166,13 @@
         <v>21</v>
       </c>
       <c r="H54" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="I54" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B55" s="10" t="s">
         <v>67</v>
       </c>
@@ -2158,7 +2195,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B56" s="10" t="s">
         <v>67</v>
       </c>
@@ -2181,7 +2218,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B57" s="10" t="s">
         <v>67</v>
       </c>
@@ -2204,7 +2241,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B58" s="10" t="s">
         <v>67</v>
       </c>
@@ -2221,13 +2258,13 @@
         <v>11</v>
       </c>
       <c r="G58" t="s">
-        <v>21</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" s="10" t="s">
         <v>67</v>
       </c>
@@ -2244,13 +2281,13 @@
         <v>11</v>
       </c>
       <c r="G59" t="s">
-        <v>21</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" s="10" t="s">
         <v>67</v>
       </c>
@@ -2273,7 +2310,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" s="10" t="s">
         <v>67</v>
       </c>
@@ -2296,7 +2333,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B62" s="10" t="s">
         <v>67</v>
       </c>
@@ -2319,7 +2356,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" s="10" t="s">
         <v>67</v>
       </c>
@@ -2342,10 +2379,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H64" s="11"/>
     </row>
-    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B65" s="12" t="s">
         <v>113</v>
       </c>
@@ -2361,11 +2398,11 @@
       <c r="G65" t="s">
         <v>21</v>
       </c>
-      <c r="H65" s="14" t="s">
+      <c r="H65" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B66" s="12" t="s">
         <v>113</v>
       </c>
@@ -2381,11 +2418,11 @@
       <c r="G66" t="s">
         <v>21</v>
       </c>
-      <c r="H66" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H66" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B67" s="12" t="s">
         <v>113</v>
       </c>
@@ -2401,11 +2438,11 @@
       <c r="G67" t="s">
         <v>21</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H67" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B68" s="12" t="s">
         <v>113</v>
       </c>
@@ -2421,11 +2458,11 @@
       <c r="G68" t="s">
         <v>21</v>
       </c>
-      <c r="H68" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H68" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B69" s="12"/>
       <c r="H69" s="2"/>
     </row>

</xml_diff>

<commit_message>
tiny change to the assest list
just ticked off a few boxes for tasks on the assest list. A few of the items are getting cut, it's important to update it.
</commit_message>
<xml_diff>
--- a/Documentation/AssetList.xlsx
+++ b/Documentation/AssetList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FroggyChainsaw\Documents\GitHub\DarkRoot\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C392764-F835-4753-97F9-92F0076A3B62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48322ADA-8FC0-4530-832C-D91092C2AD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="28800" windowHeight="15460" xr2:uid="{83EF7ABD-5B94-4EE7-81F2-F128B123CE05}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{83EF7ABD-5B94-4EE7-81F2-F128B123CE05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="124">
   <si>
     <t>Asset</t>
   </si>
@@ -201,10 +201,6 @@
 box spawns.</t>
   </si>
   <si>
-    <t>Once the dialogue box spawns, text will display on it, and the Player can click or press 'E' to advance 
-the dialogue. 'Esc' exits the dialogue.</t>
-  </si>
-  <si>
     <t>While talking to an NPC, the Player can not fire their gun or move. They are invulnerable to attack.</t>
   </si>
   <si>
@@ -408,6 +404,13 @@
   </si>
   <si>
     <t xml:space="preserve">A carrot that drops from enemies and can be found in the overworld. </t>
+  </si>
+  <si>
+    <t>Cut</t>
+  </si>
+  <si>
+    <t>Once the dialogue box spawns, text will display on it, and the Player can click or press 'E' to advance 
+the dialogue. 'Esc' exits the dialogue.(I changed Esc to spacebar, might change it back.</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3"/>
@@ -576,6 +579,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -939,7 +943,7 @@
   <dimension ref="B2:J69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,15 +961,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B3" s="1" t="s">
@@ -1467,10 +1471,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" t="s">
         <v>79</v>
-      </c>
-      <c r="D24" t="s">
-        <v>80</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
@@ -1490,10 +1494,10 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E25" t="s">
         <v>16</v>
@@ -1513,10 +1517,10 @@
         <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E26" t="s">
         <v>16</v>
@@ -1536,10 +1540,10 @@
         <v>23</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E27" t="s">
         <v>16</v>
@@ -1559,10 +1563,10 @@
         <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E28" t="s">
         <v>16</v>
@@ -1582,10 +1586,10 @@
         <v>23</v>
       </c>
       <c r="C29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E29" t="s">
         <v>16</v>
@@ -1605,10 +1609,10 @@
         <v>23</v>
       </c>
       <c r="C30" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" t="s">
         <v>93</v>
-      </c>
-      <c r="D30" t="s">
-        <v>94</v>
       </c>
       <c r="E30" t="s">
         <v>16</v>
@@ -1631,7 +1635,7 @@
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E31" t="s">
         <v>16</v>
@@ -1677,7 +1681,7 @@
         <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D34" t="s">
         <v>43</v>
@@ -1723,10 +1727,10 @@
         <v>39</v>
       </c>
       <c r="C36" t="s">
+        <v>101</v>
+      </c>
+      <c r="D36" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>103</v>
       </c>
       <c r="E36" t="s">
         <v>42</v>
@@ -1818,7 +1822,7 @@
         <v>45</v>
       </c>
       <c r="D40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E40" t="s">
         <v>42</v>
@@ -1864,7 +1868,7 @@
         <v>52</v>
       </c>
       <c r="D42" s="7" t="s">
-        <v>54</v>
+        <v>123</v>
       </c>
       <c r="E42" t="s">
         <v>42</v>
@@ -1875,8 +1879,8 @@
       <c r="G42" t="s">
         <v>21</v>
       </c>
-      <c r="H42" s="2" t="s">
-        <v>17</v>
+      <c r="H42" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.35">
@@ -1887,7 +1891,7 @@
         <v>52</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E43" t="s">
         <v>42</v>
@@ -1898,8 +1902,8 @@
       <c r="G43" t="s">
         <v>21</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>17</v>
+      <c r="H43" s="13" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.35">
@@ -1907,10 +1911,10 @@
         <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E44" t="s">
         <v>42</v>
@@ -1930,10 +1934,10 @@
         <v>39</v>
       </c>
       <c r="C45" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" t="s">
         <v>57</v>
-      </c>
-      <c r="D45" t="s">
-        <v>58</v>
       </c>
       <c r="E45" t="s">
         <v>42</v>
@@ -1953,10 +1957,10 @@
         <v>39</v>
       </c>
       <c r="C46" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" t="s">
         <v>59</v>
-      </c>
-      <c r="D46" t="s">
-        <v>60</v>
       </c>
       <c r="E46" t="s">
         <v>42</v>
@@ -1967,8 +1971,8 @@
       <c r="G46" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>17</v>
+      <c r="H46" s="14" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.35">
@@ -1976,10 +1980,10 @@
         <v>39</v>
       </c>
       <c r="C47" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D47" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E47" t="s">
         <v>42</v>
@@ -1990,8 +1994,8 @@
       <c r="G47" t="s">
         <v>21</v>
       </c>
-      <c r="H47" s="2" t="s">
-        <v>17</v>
+      <c r="H47" s="14" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.35">
@@ -1999,10 +2003,10 @@
         <v>39</v>
       </c>
       <c r="C48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" t="s">
         <v>62</v>
-      </c>
-      <c r="D48" t="s">
-        <v>63</v>
       </c>
       <c r="E48" t="s">
         <v>42</v>
@@ -2014,7 +2018,7 @@
         <v>21</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.35">
@@ -2022,10 +2026,10 @@
         <v>39</v>
       </c>
       <c r="C49" t="s">
+        <v>63</v>
+      </c>
+      <c r="D49" t="s">
         <v>64</v>
-      </c>
-      <c r="D49" t="s">
-        <v>65</v>
       </c>
       <c r="E49" t="s">
         <v>42</v>
@@ -2036,8 +2040,8 @@
       <c r="G49" t="s">
         <v>21</v>
       </c>
-      <c r="H49" s="2" t="s">
-        <v>17</v>
+      <c r="H49" s="14" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.35">
@@ -2045,10 +2049,10 @@
         <v>39</v>
       </c>
       <c r="C50" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" t="s">
         <v>97</v>
-      </c>
-      <c r="D50" t="s">
-        <v>98</v>
       </c>
       <c r="E50" t="s">
         <v>42</v>
@@ -2068,13 +2072,13 @@
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B52" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" t="s">
         <v>66</v>
       </c>
-      <c r="C52" t="s">
-        <v>67</v>
-      </c>
       <c r="D52" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E52" t="s">
         <v>42</v>
@@ -2091,13 +2095,13 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B53" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C53" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E53" t="s">
         <v>42</v>
@@ -2114,13 +2118,13 @@
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B54" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C54" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" t="s">
         <v>108</v>
-      </c>
-      <c r="D54" t="s">
-        <v>109</v>
       </c>
       <c r="E54" t="s">
         <v>42</v>
@@ -2137,13 +2141,13 @@
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B55" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C55" t="s">
+        <v>103</v>
+      </c>
+      <c r="D55" t="s">
         <v>104</v>
-      </c>
-      <c r="D55" t="s">
-        <v>105</v>
       </c>
       <c r="E55" t="s">
         <v>42</v>
@@ -2160,13 +2164,13 @@
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B56" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" t="s">
+        <v>105</v>
+      </c>
+      <c r="D56" t="s">
         <v>106</v>
-      </c>
-      <c r="D56" t="s">
-        <v>107</v>
       </c>
       <c r="E56" t="s">
         <v>42</v>
@@ -2183,13 +2187,13 @@
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B57" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C57" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" t="s">
         <v>110</v>
-      </c>
-      <c r="D57" t="s">
-        <v>111</v>
       </c>
       <c r="E57" t="s">
         <v>42</v>
@@ -2206,13 +2210,13 @@
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B58" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D58" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E58" t="s">
         <v>42</v>
@@ -2229,13 +2233,13 @@
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B59" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D59" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E59" t="s">
         <v>42</v>
@@ -2252,13 +2256,13 @@
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B60" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C60" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D60" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E60" t="s">
         <v>42</v>
@@ -2275,13 +2279,13 @@
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B61" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C61" t="s">
+        <v>76</v>
+      </c>
+      <c r="D61" t="s">
         <v>77</v>
-      </c>
-      <c r="D61" t="s">
-        <v>78</v>
       </c>
       <c r="E61" t="s">
         <v>42</v>
@@ -2298,13 +2302,13 @@
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B62" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C62" t="s">
+        <v>98</v>
+      </c>
+      <c r="D62" t="s">
         <v>99</v>
-      </c>
-      <c r="D62" t="s">
-        <v>100</v>
       </c>
       <c r="E62" t="s">
         <v>42</v>
@@ -2321,13 +2325,13 @@
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B63" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C63" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" t="s">
         <v>81</v>
-      </c>
-      <c r="D63" t="s">
-        <v>82</v>
       </c>
       <c r="E63" t="s">
         <v>42</v>
@@ -2347,13 +2351,13 @@
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B65" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C65" t="s">
         <v>112</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
         <v>113</v>
-      </c>
-      <c r="D65" t="s">
-        <v>114</v>
       </c>
       <c r="F65" t="s">
         <v>8</v>
@@ -2367,13 +2371,13 @@
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B66" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C66" t="s">
+        <v>114</v>
+      </c>
+      <c r="D66" t="s">
         <v>115</v>
-      </c>
-      <c r="D66" t="s">
-        <v>116</v>
       </c>
       <c r="F66" t="s">
         <v>10</v>
@@ -2387,13 +2391,13 @@
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B67" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C67" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D67" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F67" t="s">
         <v>11</v>
@@ -2407,13 +2411,13 @@
     </row>
     <row r="68" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B68" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C68" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D68" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F68" t="s">
         <v>12</v>

</xml_diff>